<commit_message>
w2d1&2 practice & exercises
</commit_message>
<xml_diff>
--- a/week_2/spreadsheets/day_1_practice.xlsx
+++ b/week_2/spreadsheets/day_1_practice.xlsx
@@ -439,6 +439,11 @@
           <t>Gabriel</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Rolley</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -446,6 +451,11 @@
           <t>Gabriel</t>
         </is>
       </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Smith</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -453,6 +463,11 @@
           <t>Gabriel</t>
         </is>
       </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Balenga</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -460,6 +475,11 @@
           <t>Gabriel</t>
         </is>
       </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Issac</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -467,6 +487,11 @@
           <t>Gabriel</t>
         </is>
       </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Cruise</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -474,6 +499,11 @@
           <t>Gabriel</t>
         </is>
       </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Depp</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -481,6 +511,11 @@
           <t>Gabriel</t>
         </is>
       </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Heard</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -488,11 +523,21 @@
           <t>Gabriel</t>
         </is>
       </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Qiao</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
           <t>Gabriel</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Biden</t>
         </is>
       </c>
     </row>

</xml_diff>